<commit_message>
update all files & readme
</commit_message>
<xml_diff>
--- a/SuppTables/SuppTable2.xlsx
+++ b/SuppTables/SuppTable2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Orsi\OneDriveELTE\OneDrive - elte.hu\ELTE\VEO\recombinant_detection\supplementary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eltehu-my.sharepoint.com/personal/orsolya_pipek_ttk_elte_hu/Documents/ELTE/VEO/recombinant_detection/supplementary/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C703CE19-A308-4C84-996A-D979EB71DAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SuppTable2" sheetId="1" r:id="rId1"/>
@@ -196,7 +197,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -272,10 +273,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -492,62 +493,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -570,7 +571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>174</v>
       </c>
@@ -593,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>445</v>
       </c>
@@ -616,7 +617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>733</v>
       </c>
@@ -639,7 +640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>772</v>
       </c>
@@ -662,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>832</v>
       </c>
@@ -685,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>913</v>
       </c>
@@ -708,7 +709,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1498</v>
       </c>
@@ -731,7 +732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1807</v>
       </c>
@@ -754,7 +755,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1820</v>
       </c>
@@ -777,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2037</v>
       </c>
@@ -800,7 +801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2659</v>
       </c>
@@ -823,7 +824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2749</v>
       </c>
@@ -846,7 +847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2832</v>
       </c>
@@ -869,7 +870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>3267</v>
       </c>
@@ -892,7 +893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>3428</v>
       </c>
@@ -915,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>3457</v>
       </c>
@@ -938,7 +939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3743</v>
       </c>
@@ -961,7 +962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3828</v>
       </c>
@@ -984,7 +985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>3852</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3961</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4002</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>4573</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>4878</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>4926</v>
       </c>
@@ -1122,7 +1123,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>5192</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>5230</v>
       </c>
@@ -1168,7 +1169,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>5386</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>5388</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>5648</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>5986</v>
       </c>
@@ -1260,7 +1261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>6037</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>6285</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>6286</v>
       </c>
@@ -1329,7 +1330,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>6319</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>6512</v>
       </c>
@@ -1375,7 +1376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>6513</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>6613</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>6704</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>6730</v>
       </c>
@@ -1467,7 +1468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>6954</v>
       </c>
@@ -1490,7 +1491,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>7296</v>
       </c>
@@ -1513,7 +1514,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>7424</v>
       </c>
@@ -1536,7 +1537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>7479</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>7564</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>7798</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>8139</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>8208</v>
       </c>
@@ -1651,7 +1652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>8393</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>8593</v>
       </c>
@@ -1697,7 +1698,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>8704</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>8782</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>9072</v>
       </c>
@@ -1766,7 +1767,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>9203</v>
       </c>
@@ -1789,7 +1790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>9565</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>9857</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>9870</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>10097</v>
       </c>
@@ -1881,7 +1882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>10116</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>10323</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>10634</v>
       </c>
@@ -1950,7 +1951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>10667</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>10747</v>
       </c>
@@ -1996,7 +1997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>11005</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>11230</v>
       </c>
@@ -2042,7 +2043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>11235</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>11266</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>11282</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>11308</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>11322</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>11451</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>11503</v>
       </c>
@@ -2203,7 +2204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>11521</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>11537</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>11674</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>11824</v>
       </c>
@@ -2295,7 +2296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>12049</v>
       </c>
@@ -2318,7 +2319,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>12778</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>12854</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>12964</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>13057</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>13195</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>13458</v>
       </c>
@@ -2456,7 +2457,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>13536</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>13617</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>13860</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>14407</v>
       </c>
@@ -2548,7 +2549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>14559</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>14676</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>14740</v>
       </c>
@@ -2617,7 +2618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>15009</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>15240</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>15279</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>15451</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>16176</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>16293</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>16466</v>
       </c>
@@ -2778,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>16500</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>16575</v>
       </c>
@@ -2824,7 +2825,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>17014</v>
       </c>
@@ -2847,7 +2848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>17074</v>
       </c>
@@ -2870,7 +2871,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>17259</v>
       </c>
@@ -2893,7 +2894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>17339</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>17491</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>17523</v>
       </c>
@@ -2962,7 +2963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>17707</v>
       </c>
@@ -2985,7 +2986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>17745</v>
       </c>
@@ -3008,7 +3009,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>18171</v>
       </c>
@@ -3031,7 +3032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>18395</v>
       </c>
@@ -3054,7 +3055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>18877</v>
       </c>
@@ -3077,7 +3078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>19035</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>20148</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>20396</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>20402</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>20578</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>20724</v>
       </c>
@@ -3215,7 +3216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>21255</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>21575</v>
       </c>
@@ -3261,7 +3262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>21600</v>
       </c>
@@ -3284,7 +3285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>21621</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>21717</v>
       </c>
@@ -3330,7 +3331,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>21721</v>
       </c>
@@ -3353,7 +3354,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>21786</v>
       </c>
@@ -3376,7 +3377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>21789</v>
       </c>
@@ -3399,7 +3400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>21801</v>
       </c>
@@ -3422,7 +3423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>21801</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>21895</v>
       </c>
@@ -3468,7 +3469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>21974</v>
       </c>
@@ -3491,7 +3492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>21980</v>
       </c>
@@ -3514,7 +3515,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>22000</v>
       </c>
@@ -3537,7 +3538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>22018</v>
       </c>
@@ -3560,7 +3561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>22022</v>
       </c>
@@ -3583,7 +3584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>22033</v>
       </c>
@@ -3606,7 +3607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>22132</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>22206</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>22280</v>
       </c>
@@ -3675,7 +3676,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>22298</v>
       </c>
@@ -3698,7 +3699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>22320</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>22356</v>
       </c>
@@ -3744,7 +3745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>22384</v>
       </c>
@@ -3767,7 +3768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>22599</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>22661</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>22673</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>22687</v>
       </c>
@@ -3859,7 +3860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>22812</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>22879</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>23031</v>
       </c>
@@ -3928,7 +3929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>23042</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>23202</v>
       </c>
@@ -3974,7 +3975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>23271</v>
       </c>
@@ -3997,7 +3998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>23287</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>23341</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>23401</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>23593</v>
       </c>
@@ -4089,7 +4090,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>23673</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>23709</v>
       </c>
@@ -4135,7 +4136,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>23731</v>
       </c>
@@ -4158,7 +4159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>23948</v>
       </c>
@@ -4181,7 +4182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>24097</v>
       </c>
@@ -4204,7 +4205,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>24130</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>24138</v>
       </c>
@@ -4250,7 +4251,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>24187</v>
       </c>
@@ -4273,7 +4274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>24224</v>
       </c>
@@ -4296,7 +4297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>24382</v>
       </c>
@@ -4319,7 +4320,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>24503</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>24506</v>
       </c>
@@ -4365,7 +4366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>24642</v>
       </c>
@@ -4388,7 +4389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>24748</v>
       </c>
@@ -4411,7 +4412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>24836</v>
       </c>
@@ -4434,7 +4435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>24863</v>
       </c>
@@ -4457,7 +4458,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>24893</v>
       </c>
@@ -4480,7 +4481,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>24914</v>
       </c>
@@ -4503,7 +4504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>24950</v>
       </c>
@@ -4526,7 +4527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>24977</v>
       </c>
@@ -4549,7 +4550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>25276</v>
       </c>
@@ -4572,7 +4573,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>25517</v>
       </c>
@@ -4595,7 +4596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>25517</v>
       </c>
@@ -4618,7 +4619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>25904</v>
       </c>
@@ -4641,7 +4642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>26149</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>26167</v>
       </c>
@@ -4687,7 +4688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>26305</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>26456</v>
       </c>
@@ -4733,7 +4734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>26492</v>
       </c>
@@ -4756,7 +4757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>26529</v>
       </c>
@@ -4779,7 +4780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>26530</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>26801</v>
       </c>
@@ -4825,7 +4826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>26894</v>
       </c>
@@ -4848,7 +4849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>26895</v>
       </c>
@@ -4871,7 +4872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>27204</v>
       </c>
@@ -4894,7 +4895,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>27297</v>
       </c>
@@ -4917,7 +4918,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>27752</v>
       </c>
@@ -4940,7 +4941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>27788</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>27886</v>
       </c>
@@ -4986,7 +4987,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>27889</v>
       </c>
@@ -5009,7 +5010,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>27897</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>27925</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>27970</v>
       </c>
@@ -5078,7 +5079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>27972</v>
       </c>
@@ -5101,7 +5102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>28005</v>
       </c>
@@ -5124,7 +5125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>28048</v>
       </c>
@@ -5147,7 +5148,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>28093</v>
       </c>
@@ -5170,7 +5171,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>28111</v>
       </c>
@@ -5193,7 +5194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>28144</v>
       </c>
@@ -5216,7 +5217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>28209</v>
       </c>
@@ -5239,7 +5240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>28247</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>28262</v>
       </c>
@@ -5285,7 +5286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>28270</v>
       </c>
@@ -5308,7 +5309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>28271</v>
       </c>
@@ -5331,7 +5332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>28277</v>
       </c>
@@ -5354,7 +5355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>28280</v>
       </c>
@@ -5377,7 +5378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>28281</v>
       </c>
@@ -5400,7 +5401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>28282</v>
       </c>
@@ -5423,7 +5424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>28308</v>
       </c>
@@ -5446,7 +5447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>28378</v>
       </c>
@@ -5469,7 +5470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>28461</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>28472</v>
       </c>
@@ -5515,7 +5516,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>28512</v>
       </c>
@@ -5538,7 +5539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>28628</v>
       </c>
@@ -5561,7 +5562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>28657</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>28699</v>
       </c>
@@ -5607,7 +5608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>28724</v>
       </c>
@@ -5630,7 +5631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>28742</v>
       </c>
@@ -5653,7 +5654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>28744</v>
       </c>
@@ -5676,7 +5677,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>28877</v>
       </c>
@@ -5699,7 +5700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>28878</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>28878</v>
       </c>
@@ -5745,7 +5746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>28895</v>
       </c>
@@ -5768,7 +5769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>28913</v>
       </c>
@@ -5791,7 +5792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>28932</v>
       </c>
@@ -5814,7 +5815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>28977</v>
       </c>
@@ -5837,7 +5838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>29362</v>
       </c>
@@ -5860,7 +5861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>29543</v>
       </c>
@@ -5883,7 +5884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>29645</v>
       </c>
@@ -5906,7 +5907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>29724</v>
       </c>
@@ -5929,7 +5930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>29742</v>
       </c>
@@ -5952,7 +5953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>29748</v>
       </c>
@@ -5975,7 +5976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>29754</v>
       </c>
@@ -5998,7 +5999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>29769</v>
       </c>
@@ -6021,7 +6022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>29834</v>
       </c>
@@ -6044,7 +6045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>29868</v>
       </c>

</xml_diff>